<commit_message>
book excel chýbaju 3
</commit_message>
<xml_diff>
--- a/diplomovka/moja_praca/xml_data/book_moje.xlsx
+++ b/diplomovka/moja_praca/xml_data/book_moje.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repositories\FHI\diplomovka\moja_praca\xml_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3CF186-29A6-4FC1-A33B-43FEAAD03A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96246D1A-1DCA-4883-92EA-43FC8CFB8E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14955" yWindow="5310" windowWidth="19200" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="143">
   <si>
     <t>id</t>
   </si>
@@ -254,31 +254,6 @@
   </si>
   <si>
     <t>Slovart</t>
-  </si>
-  <si>
-    <r>
-      <t>Niektoré z temných stránok nového demokratického režimu - drogy a prostitúcia - na seba nedali dlho čakať, prejavili sa krátko po revolúcii. Chlapci z oddelenia vrážd sa s nimi stretávali bežne aj predtým, no v menej drastickej podobe. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>Dnes nemali šťastie, vrah sa činil, nešetril ani ich, ani ju - mladú pouličnú prostitútku dopichal, podrezal a naaranžoval jej mŕtvolu tak, akoby ležala vystavená na márach. Ale bola naozaj podrezaná?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t> Naozaj ju vystavil, aby im chcel zanechať nejaký odkaz? Zahráva sa s nimi?</t>
-    </r>
   </si>
   <si>
     <t>Smrť na druhom brehu</t>
@@ -605,25 +580,187 @@
     <t>Prvá dáma anglickej detektívky nám vo svojom románe z roku 1927 predstavila Hercula Poirota v celkom inom, prekvapivom svetle: slávny detektív v ňom namiesto zvyčajného vyšetrovania prípadu vraždy vo vidieckom sídle zvádza súboj s mimoriadne nebezpečnou medzinárodnou organizáciou, usilujúcou sa ovládnuť svet.
 Každý osve predstavoval obrovskú hrozbu. Keď sa spojili, stali sa prakticky neporaziteľnými. Členovia Veľkej štvorky - geniálny Číňan, americký milionár, francúzska vedkyňa a nepolapiteľný majster prestrojení – zosnovali zločinecké sprisahanie takých obludných rozmerov, že šokuje i samého Poirota. V súboji s nimi mu pomáhajú jeho jedinečné deduktívne schopnosti, no čím dlhšie sa ich snaží vystopovať, tým jasnejšie sa ukazuje, že toto môže byť jeho posledný, osudný prípad...</t>
   </si>
+  <si>
+    <t>Niektoré z temných stránok nového demokratického režimu - drogy a prostitúcia - na seba nedali dlho čakať, prejavili sa krátko po revolúcii. Chlapci z oddelenia vrážd sa s nimi stretávali bežne aj predtým, no v menej drastickej podobe. Dnes nemali šťastie, vrah sa činil, nešetril ani ich, ani ju - mladú pouličnú prostitútku dopichal, podrezal a naaranžoval jej mŕtvolu tak, akoby ležala vystavená na márach. Ale bola naozaj podrezaná? Naozaj ju vystavil, aby im chcel zanechať nejaký odkaz? Zahráva sa s nimi?</t>
+  </si>
+  <si>
+    <t>Eiffel</t>
+  </si>
+  <si>
+    <t>Nicolas d'Estienne d'Orves</t>
+  </si>
+  <si>
+    <t>Spoločenská beletria</t>
+  </si>
+  <si>
+    <t>9788056630006</t>
+  </si>
+  <si>
+    <t>Lindeni,</t>
+  </si>
+  <si>
+    <t>Píše sa rok 1886 a Paríž sa pripravuje na Svetovú výstavu. Gustave Eiffel má ohromiť Francúzsko dosiaľ nevídaným monumentom, 300-metrovou vežou, ktorá bude najvyššou na svete. Je to však jediný dôvod posadnutosti kovovou stavbou, ktorá núti „básnika železa“ neúnavne a bez prestávky pracovať, rysovať plány a hľadať pre ňu dokonalý tvar?
+Ako sa hovorí, „cherchez la femme“ - za všetkým hľadaj ženu. Od opätovného stretnutia so svojou osudovou, dávno stratenou láskou akoby sa Adrienne vtelila do Eiffelovho životného projektu. Je to krivka jej chrbta, ktorá ho inšpirovala, veľké A, ktoré sa bude navždy týčiť k parížskemu nebu.</t>
+  </si>
+  <si>
+    <t>Pán prsteňov III. - Návrat kráľa</t>
+  </si>
+  <si>
+    <t>J.R.R. Tolkien</t>
+  </si>
+  <si>
+    <t>9788055606309</t>
+  </si>
+  <si>
+    <t>Pán prsteňov je rozprávkovou históriou Vojny o Prsteň, rozprávaním o boji slobodných národov Stredozeme proti Tieňu a o putovaní Hobita Froda, ktorý sa vyberie zachrániť svet. Po rozbití Spoločenstva Prsteňa a príchode Veľkej tmy začína Vojna o Prsteň, ktorá má rozhodnúť o všetkom...</t>
+  </si>
+  <si>
+    <t>Kaviareň v Kodani</t>
+  </si>
+  <si>
+    <t>Julie Caplin</t>
+  </si>
+  <si>
+    <t>9788080900946</t>
+  </si>
+  <si>
+    <t>Pripravte si šálku voňavej horúcej čokolády, natiahnite si hrubé ponožky, schúľte sa do kresla a vydajte sa spolu s hlavnou hrdinkou Katie do Kodane. Čaká vás prekvapivá cesta za povestným dánskym šťastím a... romantickou sladkou láskou.</t>
+  </si>
+  <si>
+    <t>Hotelík na Islande</t>
+  </si>
+  <si>
+    <t>9788080902650</t>
+  </si>
+  <si>
+    <t>Cosmopolis</t>
+  </si>
+  <si>
+    <t>Príbeh z krajiny ľadu a gejzírov vám ukáže, že cesta za pravou láskou je často vydláždená sklamaniami, ale aj to, že šikovný človek i napriek bolestivým zakopnutiam svoje miesto pod slnkom vždy nakoniec nájde.</t>
+  </si>
+  <si>
+    <t>Ako si získavať priateľov a pôsobiť na ľudí</t>
+  </si>
+  <si>
+    <t>Sebarozvoj</t>
+  </si>
+  <si>
+    <t>Dale Carnegie</t>
+  </si>
+  <si>
+    <t>9788055149134</t>
+  </si>
+  <si>
+    <t>Príroda,</t>
+  </si>
+  <si>
+    <t>Dale Carnegie ponúka vo svojich knihách, ktoré sa stali svetovými bestsellermi, praktické návody, ktoré môžete začať používať hneď zajtra. Táto knižka hovorí o veľkom tajomstve správneho prístupu k ľuďom, ako urobiť dobrý dojem, viesť dialóg, ako si nenarobiť nepriateľov a získať si druhých na spoluprácu.</t>
+  </si>
+  <si>
+    <t>Ako sa zbaviť starostí a začať žiť</t>
+  </si>
+  <si>
+    <t>9788055149240</t>
+  </si>
+  <si>
+    <t>Starosti vyciciavajú z človeka energiu a nedovoľujú mu premýšľať. Môžeme urobiť niečo, aby sme sa ich zbavili? Dale Carnegie v tejto knihe dokazuje, že je to možné. Ponúka overené techniky, ktoré už miliónom ľudí na celom svete pomohli zmeniť ich život. Pomocou praktických návodov sa aj vy naučíte riešiť problematické situácie, využiť kritiku vo svoj prospech či vyhnúť sa citovému rozrušeniu. Autor vám poradí, ako si vypestovať duševný postoj, z ktorého pramení pokoj a šťastie, ale aj pracovné návyky, ktoré pomáhajú zabraňovať únave.</t>
+  </si>
+  <si>
+    <t>Diana</t>
+  </si>
+  <si>
+    <t>Andrew Morton</t>
+  </si>
+  <si>
+    <t>Životopisy</t>
+  </si>
+  <si>
+    <t>Universum</t>
+  </si>
+  <si>
+    <t>Kniha Diana, její skutečný příběh po svém prvním vydání v roce 1992 navždy změnila způsob, jakým veřejnost pohlížela na britskou monarchii. Na prvním místě žebříčku bestsellerů deníku New York Times se stala unikátní literární klasikou nejen pro svůj výbušný obsah, ale i proto, že se Diana na publikaci osobně podílela.</t>
+  </si>
+  <si>
+    <t>Steve Jobs</t>
+  </si>
+  <si>
+    <t>Walter Isaacson</t>
+  </si>
+  <si>
+    <t>Skutočnú pravdu o ikone úspechu novodobej technologickej éry a jeho fenomenálnej spoločnosti Apple sa dozvedia čitatelia v slovenskom vydaní autobiografickej knihy STEVE JOBS, ktorú vydáva vydavateľstvo Eastone Books vo svojej edícii Business Class. Steve Jobs významne ovplyvnil vývoj osobných počítačov, kreslených filmov, telefónov, hudby, tabletov a digitálnej tlače.
+Autorom unikátneho životopisu Stevea Jobsa je renomovaný novinár a publicista Walter Isaacson, bývalý predseda predstavenstva a CEO televíznej stanice CNN a niekdajší šéfredaktor časopisu Time Magazine.
+Médiá sa neustále predbiehajú v tom, kto prvý prinesie „nové a zaručené“ informácie o tejto „technologickej popstar“ a jeho trendy určujúcej spoločnosti Apple. Steve Jobs je prezentovaný ako charizmatický vizionár, talentovaný podnikateľ a vynaliezavý inovátor s citom pre trhové trendy. Je oslavovaný a zatracovaný zároveň. Neustály informačný „boom“ okolo osoby Stevea Jobsa a spoločnosti Apple neraz sprevádzajú aj polopravdy, mýty a účelové dezinformácie. Jedno je však nesporné. Na hviezdnom úspechu v súčasnosti najhodnotnejšej IT firmy na svete sa najväčšou mierou podieľal práve Steve Jobs. On jediný poznal skutočnú pravdu v pozadí pomyselného „Apple kódu“.
+Autor Walter Isaacson ponúka v knihe s prostým názvom STEVE JOBS výnimočný pohľad na Jobsov pracovný a súkromný život zároveň. Knižný portrét je výsledkom trojročnej práce založenej na exkluzívnych rozhovoroch a stretnutiach so samotným Jobsom, s členmi jeho rodiny, Jobsovými kolegami z Applu, ako aj s jeho konkurentmi.
+Ak teda patríte k oddaným fanúšikom všetkého, čo má na sebe logo odhryznutého jabĺčka, ak premýšľate o vhodnom dare pre obchodných partnerov alebo pre niekoho blízkeho, kto je vyznávačom kultovej značky Apple alebo vás jednoducho len priťahujú príbehy úspešných biznismenov, ich vizionárske rozmýšľanie a nekonvenčné postoje, určite by ste si túto knižnú udalosť roka nemali nechať ujsť.
+Prečítajte si článok o Steveovi Jobsovi a o jeho dlho očakávanom životopise na našom blogu!
+Rozsah strán: 546 +16 strán obrazovej prílohy</t>
+  </si>
+  <si>
+    <t>Šlabikár financií pre neziskovky</t>
+  </si>
+  <si>
+    <t>9788097029135</t>
+  </si>
+  <si>
+    <t>Publikácia, ktorú práve držíte v rukách je určená všetkým, ktorí chcú založiť niektorý z typov neziskových organizácií a tiež tým, ktorí v rámci existujúcich prichádzajú do kontaktu s finančnými prostriedkami.</t>
+  </si>
+  <si>
+    <t>Malý princ</t>
+  </si>
+  <si>
+    <t>Antoine De Saint-Exupéry</t>
+  </si>
+  <si>
+    <t>klasika</t>
+  </si>
+  <si>
+    <t>9788010034666</t>
+  </si>
+  <si>
+    <t>Mladé letá</t>
+  </si>
+  <si>
+    <t>Pôvabná knižka nielen pre deti, ale pre všetkých, ktorí chcú deťom porozumieť. Toto dielko dosiahlo svetový úspech a patrí do zlatého fondu svetovej literatúry. Jeho hodnota a krása nespočíva len v peknom rozprávkovom príbehu, ale hlavne v myšlienkach, ktoré ako vzácne kamienky vytvárajú obraz ľudských vlastností...
+Saint-Exupéry svoju knižku s čistým detským pohľadom na svet venoval najlepšiemu priateľovi. Veď všetci dospelí boli najprv deťmi. Ale máloktorý z nich sa na to pamätá.</t>
+  </si>
+  <si>
+    <t>George Orwell</t>
+  </si>
+  <si>
+    <t>Nové vydanie románu 1984 - jedného z najznámejších diel svetovej literatúry. Spája v sebe prvky spoločensko-politického a vedecko-fantastického románu. Je obžalobou komunistickej diktatúry, ktorá roku 1984 ovládla všetko, vrátane ľudského myslenia. Román opisuje osudy čestného, citlivého a uvažujúceho jednotlivca (Winstona Smitha), ktorý sa vzoprie systému, za čo platí krutú daň.</t>
+  </si>
+  <si>
+    <t>Friedrich Nietzsche</t>
+  </si>
+  <si>
+    <t>Filozofia</t>
+  </si>
+  <si>
+    <t>Mimo dobro a zlo</t>
+  </si>
+  <si>
+    <t>OIKOYMENH</t>
+  </si>
+  <si>
+    <t>Německý originál knihy Mimo dobro a zlo. Předehra k filosofii budoucnosti (Jenseits von Gut und Böse. Vorspiel einer Philosophie der Zukunft) byl poprvé publikován v Lipsku roku 1886 autorovým vlastním nákladem. Kniha tedy vyšla bezprostředně po Tak pravil Zarathustra (1883-1885), ale materiál k ní shromažďoval Nietzsche už od začátku 80. let, čerpaje z poznámek zapsaných dokonce i před vydáním Radostné vědy (1882). </t>
+  </si>
+  <si>
+    <t>Co znamená myslet?</t>
+  </si>
+  <si>
+    <t>Martin Heidegger</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -657,14 +794,6 @@
       <charset val="238"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="24"/>
       <color rgb="FF000000"/>
@@ -673,26 +802,19 @@
       <charset val="238"/>
     </font>
     <font>
-      <b/>
-      <sz val="26"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -714,56 +836,47 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextové prepojenie" xfId="1" builtinId="8"/>
@@ -1045,16 +1158,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:N29"/>
+  <dimension ref="B3:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
@@ -1063,11 +1176,12 @@
     <col min="10" max="10" width="20.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" customWidth="1"/>
     <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
     <col min="14" max="14" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -1108,732 +1222,1204 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5">
+    <row r="5" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="10">
         <v>1</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="10">
         <v>360</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="10">
         <v>2015</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="22" t="s">
+      <c r="M5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="10">
         <v>4.7</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6">
+    <row r="6" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
         <v>2</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="10">
         <v>712</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="10">
         <v>2015</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="20">
+      <c r="L6" s="12">
         <v>16.11</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="10">
         <v>4.8</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7">
+    <row r="7" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="10">
         <v>3</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="10">
         <v>165</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="10">
         <v>2022</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="20"/>
-      <c r="M7" s="18" t="s">
+      <c r="L7" s="12"/>
+      <c r="M7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="10">
         <v>4.5</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="8" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
         <v>4</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="10">
         <v>200</v>
       </c>
       <c r="I8" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="10">
         <v>2020</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="16">
         <v>16.559999999999999</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="M8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="10">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9">
+    <row r="9" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="10">
         <v>5</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="10">
         <v>256</v>
       </c>
       <c r="I9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="10">
         <v>2022</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="21" t="s">
+      <c r="L9" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="M9" s="13" t="s">
+      <c r="M9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="10">
         <v>4.7</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="10" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
         <v>6</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="10">
         <v>315</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="10">
         <v>2017</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="L10" s="20" t="s">
+      <c r="L10" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="M10" s="13" t="s">
+      <c r="M10" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="10">
         <v>4.2</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B11">
+    <row r="11" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
         <v>7</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="10">
         <v>296</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="10">
         <v>2016</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="10">
         <v>12.79</v>
       </c>
-      <c r="M11" s="13" t="s">
+      <c r="M11" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="10">
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="12" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B12">
+    <row r="12" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
         <v>8</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="10">
         <v>424</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="10">
         <v>2020</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="10">
         <v>17.809999999999999</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="10">
         <v>4.3</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B13">
+    <row r="13" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="10">
         <v>9</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="10">
         <v>296</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="M13" s="13" t="s">
+      <c r="M13" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="10">
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="14" spans="2:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="B14">
+    <row r="14" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="10">
         <v>10</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="10">
         <v>8072267698</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="10">
         <v>360</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="10">
         <v>2003</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="10">
         <v>9.42</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="M14" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B15">
+    <row r="15" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="10">
         <v>11</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="10">
         <v>352</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="10">
         <v>2022</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="14">
         <v>12.75</v>
       </c>
-      <c r="M15" s="6" t="s">
+      <c r="M15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="N15" s="10">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="10">
+        <v>12</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="N15">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>12</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="G16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="10">
         <v>320</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="10">
         <v>2016</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="10">
         <v>13.21</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="N16" s="10">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="10">
+        <v>13</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="N16">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>13</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" t="s">
+      <c r="F17" s="15"/>
+      <c r="G17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="10">
         <v>312</v>
       </c>
       <c r="I17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="10">
         <v>2009</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="10">
         <v>14.95</v>
       </c>
-      <c r="M17" s="7" t="s">
+      <c r="M17" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="N17" s="10">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="10">
+        <v>14</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="N17" s="24">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>14</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="D18" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="G18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="10">
         <v>232</v>
       </c>
       <c r="I18" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="10">
         <v>2020</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" s="10">
+        <v>13.9</v>
+      </c>
+      <c r="M18" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="L18">
-        <v>13.9</v>
-      </c>
-      <c r="M18" s="7" t="s">
+      <c r="N18" s="10">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="10">
+        <v>15</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="N18">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B19">
+      <c r="D19" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="2">
+      <c r="H19" s="10">
         <v>184</v>
       </c>
       <c r="I19" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="10">
         <v>2019</v>
       </c>
-      <c r="K19" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="L19">
+      <c r="K19" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="L19" s="10">
         <v>10.9</v>
       </c>
-      <c r="M19" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20">
+      <c r="M19" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="N19" s="10">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="10">
         <v>16</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21">
+      <c r="C20" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="10">
+        <v>256</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="10">
+        <v>2022</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="L20" s="10">
+        <v>14.49</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="N20" s="10">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="10">
         <v>17</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22">
+      <c r="C21" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="10">
+        <v>432</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="10">
+        <v>2012</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="L21" s="10">
+        <v>14.46</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="N21" s="10">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="7">
         <v>18</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23">
+      <c r="C22" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="10">
+        <v>352</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="10">
+        <v>2020</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L22" s="10">
+        <v>13.99</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="N22" s="10">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7">
         <v>19</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24">
+      <c r="C23" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="10">
+        <v>344</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="10">
+        <v>2022</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="L23" s="10">
+        <v>14.17</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="N23" s="10">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="7">
         <v>20</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25">
+      <c r="C24" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="10">
+        <v>256</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="10">
+        <v>2016</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="L24" s="10">
+        <v>12.9</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="N24" s="10">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="7">
         <v>21</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26">
+      <c r="C25" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="7">
+        <v>320</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="7">
+        <v>2016</v>
+      </c>
+      <c r="K25" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="L25" s="7">
+        <v>12.9</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="N25" s="7">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="7">
         <v>22</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27">
+      <c r="C26" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" s="2">
+        <v>9788024275925</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="7">
+        <v>400</v>
+      </c>
+      <c r="I26" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28">
+      <c r="J26" s="7">
+        <v>2022</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="L26" s="7">
+        <v>22.58</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="N26" s="7">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="7">
+        <v>23</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F27" s="2">
+        <v>9788081091940</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="7">
+        <v>562</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="7">
+        <v>2011</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L27" s="7">
+        <v>22.55</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="N27" s="7">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="7">
         <v>24</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29">
+      <c r="C28" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="7">
+        <v>137</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="7">
+        <v>2022</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L28" s="7">
+        <v>14.2</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="N28" s="7">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="7">
         <v>25</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="F29" s="3"/>
+      <c r="C29" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="7">
+        <v>253</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" s="7">
+        <v>2019</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="L29" s="7">
+        <v>4.79</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="N29" s="7">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="7">
+        <v>26</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1984</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="7">
+        <v>9788055610832</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="7">
+        <v>253</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="7">
+        <v>2013</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L30" s="7">
+        <v>12.95</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="N30" s="7">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="7">
+        <v>27</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F31" s="7">
+        <v>9788072985852</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="7">
+        <v>223</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" s="7">
+        <v>2021</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="L31" s="7">
+        <v>16.36</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="N31" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="7">
+        <v>28</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F32" s="7">
+        <v>9788072984947</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="7">
+        <v>60</v>
+      </c>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+    </row>
+    <row r="33" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="7">
+        <v>29</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+    </row>
+    <row r="34" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="7">
+        <v>30</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I6" r:id="rId1" display="https://www.martinus.sk/l?categories%5B0%5D=6003&amp;bindings%5B%5D=294829" xr:uid="{2D8F8964-5C85-4F09-A1CF-67FB51ED65A2}"/>
-    <hyperlink ref="E5" r:id="rId2" display="https://www.martinus.sk/l?categories%5B0%5D=6007" xr:uid="{33694406-E44E-4270-BD26-0F4C804C713D}"/>
-    <hyperlink ref="E6" r:id="rId3" display="https://www.martinus.sk/l?categories%5B0%5D=6007" xr:uid="{A6572C2B-4390-4F31-A4AE-8964F0992BED}"/>
-    <hyperlink ref="D7" r:id="rId4" display="https://www.martinus.sk/authors/jaroslava-lukacovicova" xr:uid="{0F7A3C37-2A6B-478B-B4F8-B9CD58AB631B}"/>
-    <hyperlink ref="E7" r:id="rId5" display="https://www.martinus.sk/l?categories%5B0%5D=6206" xr:uid="{9685794C-8224-4F19-AFA5-48B9090E5B9E}"/>
-    <hyperlink ref="I7" r:id="rId6" display="https://www.martinus.sk/l?categories%5B0%5D=6212&amp;bindings%5B%5D=294829" xr:uid="{CC9C7C2C-5F9E-4078-83C5-60840D6C5CBA}"/>
-    <hyperlink ref="K7" r:id="rId7" display="https://www.martinus.sk/knihy/vydavatelstvo/sauno" xr:uid="{62CC61F7-B2A9-4F58-84A5-32FCA5D45468}"/>
-    <hyperlink ref="D8" r:id="rId8" display="https://www.martinus.sk/authors/karolina-fourova" xr:uid="{50F6B1CC-EBBF-495E-B841-8B9E721D7E54}"/>
-    <hyperlink ref="E8" r:id="rId9" display="https://www.martinus.sk/l?categories%5B0%5D=6742" xr:uid="{9B998212-383B-4BCC-894A-D35D638EF9A7}"/>
-    <hyperlink ref="I8" r:id="rId10" display="https://www.martinus.sk/l?categories%5B0%5D=6212&amp;bindings%5B%5D=294829" xr:uid="{92BB2075-E4B9-4A9E-B0E9-F74FE3732CBF}"/>
-    <hyperlink ref="K8" r:id="rId11" display="https://www.martinus.sk/knihy/vydavatelstvo/esence" xr:uid="{C36BEC59-B843-4D2E-A723-8E4F9D981908}"/>
-    <hyperlink ref="D9" r:id="rId12" display="https://www.martinus.sk/authors/arthur-c-clarke" xr:uid="{02F4ED55-3AC4-44D1-B121-D54364F618B5}"/>
-    <hyperlink ref="E9" r:id="rId13" display="https://www.martinus.sk/l?categories%5B0%5D=6087" xr:uid="{0EF1065D-90D7-4DFE-9433-15B41D48E584}"/>
-    <hyperlink ref="I9" r:id="rId14" display="https://www.martinus.sk/l?categories%5B0%5D=6212&amp;bindings%5B%5D=294829" xr:uid="{35CA28DD-856A-4A37-B417-562D4CE908EF}"/>
-    <hyperlink ref="K9" r:id="rId15" display="https://www.martinus.sk/knihy/vydavatelstvo/argo" xr:uid="{089649F1-0536-4F2A-8D93-7C1E264A9F57}"/>
-    <hyperlink ref="D10" r:id="rId16" display="https://www.martinus.sk/authors/arthur-c-clarke" xr:uid="{66CF7FBA-ACDB-40DB-8F86-9F60FBE43271}"/>
-    <hyperlink ref="E10" r:id="rId17" display="https://www.martinus.sk/l?categories%5B0%5D=6087" xr:uid="{29EA1A18-F390-4359-98C8-BE1C27726F65}"/>
-    <hyperlink ref="I10" r:id="rId18" display="https://www.martinus.sk/l?categories%5B0%5D=6212&amp;bindings%5B%5D=294829" xr:uid="{DF96DC1A-8FD9-4317-B335-7682D5CAB953}"/>
-    <hyperlink ref="K10" r:id="rId19" display="https://www.martinus.sk/knihy/vydavatelstvo/argo" xr:uid="{66C2F274-3A7D-476C-8E2B-FD95DA08C225}"/>
-    <hyperlink ref="E11" r:id="rId20" display="https://www.martinus.sk/l?categories%5B0%5D=6746" xr:uid="{7A0F616A-87BD-4107-ACB3-91C047167A4C}"/>
-    <hyperlink ref="D12" r:id="rId21" display="https://www.martinus.sk/authors/miroslav-virius" xr:uid="{7BF11037-3CD0-484D-AE72-CD2495FA06F9}"/>
-    <hyperlink ref="E12" r:id="rId22" display="https://www.martinus.sk/l?categories%5B0%5D=6746" xr:uid="{C7F405E6-44D1-44D9-8CFE-916360980146}"/>
-    <hyperlink ref="I11" r:id="rId23" display="https://www.martinus.sk/l?categories%5B0%5D=6212&amp;bindings%5B%5D=294829" xr:uid="{B21D9A00-AB56-48E5-887D-120313EF0A61}"/>
-    <hyperlink ref="K12" r:id="rId24" display="https://www.martinus.sk/knihy/vydavatelstvo/grada" xr:uid="{B7DE032A-95C8-4303-93D0-99B933F69D0E}"/>
-    <hyperlink ref="D11" r:id="rId25" display="https://www.martinus.sk/authors/michaela-sebokova-vannini" xr:uid="{B2A83CA6-CF26-47DC-8EE6-A364602C35D5}"/>
-    <hyperlink ref="D13" r:id="rId26" display="https://www.martinus.sk/authors/mike-shema" xr:uid="{AC5D4B02-91AC-4F87-BB0F-AAA92AB3DD23}"/>
-    <hyperlink ref="E13" r:id="rId27" display="https://www.martinus.sk/l?categories%5B0%5D=6746" xr:uid="{B01612F5-43D3-4D99-BB96-EB5D02E48543}"/>
-    <hyperlink ref="K13" r:id="rId28" display="https://www.martinus.sk/knihy/vydavatelstvo/syngress" xr:uid="{C07B9D24-B0A6-4FA6-8EBC-48CA57B9B426}"/>
-    <hyperlink ref="D14" r:id="rId29" display="https://www.martinus.sk/authors/mike-shema" xr:uid="{35722ABC-5625-4698-B358-CADD537F1BFF}"/>
-    <hyperlink ref="E14" r:id="rId30" display="https://www.martinus.sk/l?categories%5B0%5D=6746" xr:uid="{BC8F3238-47C6-4D5F-AE83-5FF77F87CFCA}"/>
-    <hyperlink ref="K14" r:id="rId31" display="https://www.martinus.sk/knihy/vydavatelstvo/computer-press" xr:uid="{042C6932-DFC1-41CE-B963-C4DEC92992D5}"/>
-    <hyperlink ref="C15" r:id="rId32" display="https://www.martinus.sk/knihy/najpredavanejsie/" xr:uid="{4E467BCD-7CAA-4B16-B93D-1979C3186325}"/>
-    <hyperlink ref="D15" r:id="rId33" display="https://www.martinus.sk/authors/dominik-dan" xr:uid="{C445ED91-1C82-45A0-8C82-A68D69847B89}"/>
-    <hyperlink ref="E15" r:id="rId34" display="https://www.martinus.sk/l?categories%5B0%5D=6079" xr:uid="{B858BC7B-BE1C-4475-B8F1-02FD222CF1B1}"/>
-    <hyperlink ref="I15" r:id="rId35" display="https://www.martinus.sk/l?categories%5B0%5D=6212&amp;bindings%5B%5D=294829" xr:uid="{3AFD5F1D-7011-4FD0-B6FB-DABCB56F0EB1}"/>
-    <hyperlink ref="K15" r:id="rId36" display="https://www.martinus.sk/knihy/vydavatelstvo/slovart" xr:uid="{3AEC66EB-4D3E-4150-A7C3-E96ECDE8D4A8}"/>
-    <hyperlink ref="D16" r:id="rId37" display="https://www.martinus.sk/authors/dominik-dan" xr:uid="{59AC70E4-002B-40A8-9574-62CAD4A3C68D}"/>
-    <hyperlink ref="E16" r:id="rId38" display="https://www.martinus.sk/l?categories%5B0%5D=6079" xr:uid="{819C196A-DAE2-4523-9D46-A0BC6B3A68A2}"/>
-    <hyperlink ref="I16" r:id="rId39" display="https://www.martinus.sk/l?categories%5B0%5D=6212&amp;bindings%5B%5D=294829" xr:uid="{568E9290-4FE6-4CFF-AA87-F59A2E6E2BBE}"/>
-    <hyperlink ref="K16" r:id="rId40" display="https://www.martinus.sk/knihy/vydavatelstvo/slovart" xr:uid="{329758DE-F580-4D6A-8E63-F2E400F00E52}"/>
-    <hyperlink ref="D17" r:id="rId41" display="https://www.martinus.sk/authors/dominik-dan" xr:uid="{95D86543-DDF4-4A2C-BC0D-2F2EA2FAFB99}"/>
-    <hyperlink ref="E17" r:id="rId42" display="https://www.martinus.sk/l?categories%5B0%5D=6079" xr:uid="{3CD23C94-FC85-4E83-AFCB-383F72E0775F}"/>
-    <hyperlink ref="I17" r:id="rId43" display="https://www.martinus.sk/l?categories%5B0%5D=6212&amp;bindings%5B%5D=294829" xr:uid="{F4AB198E-9B02-49E0-8611-9B18173DB50F}"/>
-    <hyperlink ref="K17" r:id="rId44" display="https://www.martinus.sk/knihy/vydavatelstvo/slovart" xr:uid="{3103DBC6-BB4C-4268-8185-21DD3C7F3F20}"/>
-    <hyperlink ref="D18" r:id="rId45" display="https://www.martinus.sk/authors/agatha-christie" xr:uid="{6DA68831-43D9-40F2-B652-2DF7C726ECB6}"/>
-    <hyperlink ref="E18" r:id="rId46" display="https://www.martinus.sk/l?categories%5B0%5D=6079" xr:uid="{C805E710-3A64-40EB-87D0-D61D50936A1C}"/>
-    <hyperlink ref="I18" r:id="rId47" display="https://www.martinus.sk/l?categories%5B0%5D=6212&amp;bindings%5B%5D=294829" xr:uid="{285126BF-D592-43B0-BC23-6477D87088A1}"/>
-    <hyperlink ref="K18" r:id="rId48" display="https://www.martinus.sk/knihy/vydavatelstvo/slovensky-spisovatel" xr:uid="{D8758F0F-4F84-4EB8-9D05-3175802C7944}"/>
-    <hyperlink ref="D19" r:id="rId49" display="https://www.martinus.sk/authors/agatha-christie" xr:uid="{D8B8E9A7-068F-4189-A594-232DAC22F5F0}"/>
-    <hyperlink ref="E19" r:id="rId50" display="https://www.martinus.sk/l?categories%5B0%5D=6079" xr:uid="{5EE9B078-77DB-4B36-828B-D163EDCB0194}"/>
-    <hyperlink ref="I19" r:id="rId51" display="https://www.martinus.sk/l?categories%5B0%5D=6212&amp;bindings%5B%5D=294829" xr:uid="{94999BBA-3E34-4513-9FA3-D54463BA76D9}"/>
-    <hyperlink ref="K19" r:id="rId52" display="https://www.martinus.sk/knihy/vydavatelstvo/slovensky-spisovatel" xr:uid="{4E0434D9-49DE-4DB9-8992-7CF8CBED6408}"/>
+    <hyperlink ref="K21" r:id="rId1" display="https://www.martinus.sk/knihy/vydavatelstvo/slovart" xr:uid="{4AE8D525-7770-4F34-9A04-5166B871DE3E}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.martinus.sk/authors/julie-caplin" xr:uid="{C83DB2C8-AAF3-44FC-BC5A-7FBBFFC2C4EF}"/>
+    <hyperlink ref="E22" r:id="rId3" display="https://www.martinus.sk/l?categories%5B0%5D=6069" xr:uid="{8B414675-27EA-4E3C-B85A-2940ED922D42}"/>
+    <hyperlink ref="I22" r:id="rId4" display="https://www.martinus.sk/l?categories%5B0%5D=6069&amp;bindings%5B%5D=294831" xr:uid="{7A9CD9F2-BC97-45A0-977C-4C7FC92C883C}"/>
+    <hyperlink ref="K22" r:id="rId5" display="https://www.martinus.sk/knihy/vydavatelstvo/grada" xr:uid="{80E37186-57D7-4907-8AFE-AA84AA625028}"/>
+    <hyperlink ref="D23" r:id="rId6" display="https://www.martinus.sk/authors/julie-caplin" xr:uid="{5DD363A3-DDC7-4A52-ACE7-26DB23B81606}"/>
+    <hyperlink ref="E23" r:id="rId7" display="https://www.martinus.sk/l?categories%5B0%5D=6069" xr:uid="{2F017241-EBD4-475E-8CD3-3AB23E4CAC03}"/>
+    <hyperlink ref="I23" r:id="rId8" display="https://www.martinus.sk/l?categories%5B0%5D=6069&amp;bindings%5B%5D=294831" xr:uid="{750A119C-5622-4AD1-BABC-C7D4A2E08404}"/>
+    <hyperlink ref="K23" r:id="rId9" display="https://www.martinus.sk/knihy/vydavatelstvo/cosmopolis" xr:uid="{74D1E67E-3EFF-46DF-BC2D-530DD967C185}"/>
+    <hyperlink ref="E24" r:id="rId10" display="https://www.martinus.sk/l?categories%5B0%5D=6476" xr:uid="{8E198BD9-F862-4619-855F-F7F55324B3A9}"/>
+    <hyperlink ref="D24" r:id="rId11" display="https://www.martinus.sk/authors/dale-carnegie" xr:uid="{D63CF761-A382-4E55-A0EC-8A193564907F}"/>
+    <hyperlink ref="K24" r:id="rId12" display="https://www.martinus.sk/knihy/vydavatelstvo/priroda" xr:uid="{66EFAF95-3046-4C30-B9CF-2C50B90D7CEE}"/>
+    <hyperlink ref="D25" r:id="rId13" display="https://www.martinus.sk/authors/dale-carnegie" xr:uid="{261C3ABB-19A4-4FCB-8A4A-E376DB4E5A9E}"/>
+    <hyperlink ref="E25" r:id="rId14" display="https://www.martinus.sk/l?categories%5B0%5D=6476" xr:uid="{7E851D28-B38C-4486-BBE0-A9B23A67B948}"/>
+    <hyperlink ref="K25" r:id="rId15" display="https://www.martinus.sk/knihy/vydavatelstvo/priroda" xr:uid="{B22447E8-7350-4F51-BF2B-1EB3FD677640}"/>
+    <hyperlink ref="D26" r:id="rId16" display="https://www.martinus.sk/authors/andrew-morton" xr:uid="{E523F735-1118-4C08-A6F4-B9E4BA4477DB}"/>
+    <hyperlink ref="E26" r:id="rId17" display="https://www.martinus.sk/l?categories%5B0%5D=7890" xr:uid="{A878716B-1ADC-4ADA-AC58-5D3F008B66C2}"/>
+    <hyperlink ref="K26" r:id="rId18" display="https://www.martinus.sk/knihy/vydavatelstvo/universum" xr:uid="{6AEDB845-5D33-4CF9-976A-0C76BF6667F3}"/>
+    <hyperlink ref="D27" r:id="rId19" display="https://www.martinus.sk/authors/walter-isaacson" xr:uid="{1CA5D7C1-7B5A-4956-8D08-34F62937B5FE}"/>
+    <hyperlink ref="E27" r:id="rId20" display="https://www.martinus.sk/l?categories%5B0%5D=7890" xr:uid="{B65E0675-2FBF-481D-B3F3-3D4ECB47A8D3}"/>
+    <hyperlink ref="K27" r:id="rId21" display="https://www.martinus.sk/knihy/vydavatelstvo/eastone-books" xr:uid="{9A22C79F-A6FC-4FA1-A793-88B96616340E}"/>
+    <hyperlink ref="D28" r:id="rId22" display="https://www.martinus.sk/authors/jaroslava-lukacovicova" xr:uid="{643C2BB3-7B63-41B0-B06D-91B180FA1318}"/>
+    <hyperlink ref="K28" r:id="rId23" display="https://www.martinus.sk/knihy/vydavatelstvo/sauno" xr:uid="{CF996D13-EC9E-441E-9D8F-D91BF2F658B0}"/>
+    <hyperlink ref="C29" r:id="rId24" display="https://www.martinus.sk/knihy/najpredavanejsie/" xr:uid="{DDACB427-6565-4B73-8743-459F03F58913}"/>
+    <hyperlink ref="D29" r:id="rId25" display="https://www.martinus.sk/authors/antoine-de-saint-exupery-3" xr:uid="{4A68BEB7-5B5A-4A3D-9247-7B3E07F37458}"/>
+    <hyperlink ref="K29" r:id="rId26" display="https://www.martinus.sk/knihy/vydavatelstvo/spn-mlade-leta" xr:uid="{96263DF7-14E7-4D9D-AF05-192652026D3B}"/>
+    <hyperlink ref="D30" r:id="rId27" display="https://www.martinus.sk/authors/george-orwell" xr:uid="{DFABF9BA-8DB8-4DDA-97D0-DEB2B4A04AC7}"/>
+    <hyperlink ref="K30" r:id="rId28" display="https://www.martinus.sk/knihy/vydavatelstvo/slovart" xr:uid="{93247411-9A71-475F-9C91-21807D66FEB9}"/>
+    <hyperlink ref="D31" r:id="rId29" display="https://www.martinus.sk/authors/friedrich-nietzsche" xr:uid="{F6003EC7-52FA-4019-BAA1-42C4108DA753}"/>
+    <hyperlink ref="E31" r:id="rId30" display="https://www.martinus.sk/l?categories%5B0%5D=6308" xr:uid="{7B11D5EC-7FEB-4D45-8214-AE244C6559F7}"/>
+    <hyperlink ref="I31" r:id="rId31" display="https://www.martinus.sk/l?categories%5B0%5D=6308&amp;bindings%5B%5D=294829" xr:uid="{837CB111-0739-4A63-95DD-539FDF849E50}"/>
+    <hyperlink ref="K31" r:id="rId32" display="https://www.martinus.sk/knihy/vydavatelstvo/oikoymenh" xr:uid="{5BA79861-FFE1-4D53-AC6B-F5DB34D04D21}"/>
+    <hyperlink ref="D32" r:id="rId33" display="https://www.martinus.sk/authors/martin-heidegger" xr:uid="{0588E036-9A37-4523-85C9-0D9371B8529F}"/>
+    <hyperlink ref="E32" r:id="rId34" display="https://www.martinus.sk/l?categories%5B0%5D=6308" xr:uid="{4DF89998-37C8-4F18-A27A-364E1CC99D10}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>